<commit_message>
Mejoras en los gráficos
</commit_message>
<xml_diff>
--- a/models/all_baseline_data.xlsx
+++ b/models/all_baseline_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="42">
   <si>
     <t>Set</t>
   </si>
@@ -127,10 +127,10 @@
     <t>BERT</t>
   </si>
   <si>
-    <t>TeRCEx</t>
+    <t>ETeR-X</t>
   </si>
   <si>
-    <t>BiVAECF</t>
+    <t>BiVAE</t>
   </si>
   <si>
     <t>EASEᴿ</t>
@@ -140,78 +140,6 @@
   </si>
   <si>
     <t>USEM</t>
-  </si>
-  <si>
-    <t>28.6884</t>
-  </si>
-  <si>
-    <t>1.0422</t>
-  </si>
-  <si>
-    <t>352.6678</t>
-  </si>
-  <si>
-    <t>12.4069</t>
-  </si>
-  <si>
-    <t>411.1219</t>
-  </si>
-  <si>
-    <t>18.1851</t>
-  </si>
-  <si>
-    <t>1439.7406</t>
-  </si>
-  <si>
-    <t>33.7482</t>
-  </si>
-  <si>
-    <t>997.8453</t>
-  </si>
-  <si>
-    <t>27.9478</t>
-  </si>
-  <si>
-    <t>69.3459</t>
-  </si>
-  <si>
-    <t>3.4404</t>
-  </si>
-  <si>
-    <t>100.5543</t>
-  </si>
-  <si>
-    <t>4.3565</t>
-  </si>
-  <si>
-    <t>40.1660</t>
-  </si>
-  <si>
-    <t>2.4810</t>
-  </si>
-  <si>
-    <t>52.8296</t>
-  </si>
-  <si>
-    <t>3.4475</t>
-  </si>
-  <si>
-    <t>43.1859</t>
-  </si>
-  <si>
-    <t>2.1179</t>
-  </si>
-  <si>
-    <t>345.8308</t>
-  </si>
-  <si>
-    <t>5.1412</t>
-  </si>
-  <si>
-    <t>386.5587</t>
-  </si>
-  <si>
-    <t>4.7858</t>
   </si>
 </sst>
 </file>
@@ -873,8 +801,8 @@
       <c r="V4">
         <v>0.2875550090046042</v>
       </c>
-      <c r="W4" t="s">
-        <v>42</v>
+      <c r="W4">
+        <v>28.6884</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -944,8 +872,8 @@
       <c r="V5">
         <v>0.2869592484067173</v>
       </c>
-      <c r="W5" t="s">
-        <v>43</v>
+      <c r="W5">
+        <v>1.0422</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1323,8 +1251,8 @@
       <c r="V10">
         <v>0.0693344707864904</v>
       </c>
-      <c r="W10" t="s">
-        <v>44</v>
+      <c r="W10">
+        <v>352.6678</v>
       </c>
     </row>
     <row r="11" spans="1:25">
@@ -1394,8 +1322,8 @@
       <c r="V11">
         <v>0.1055464416879935</v>
       </c>
-      <c r="W11" t="s">
-        <v>45</v>
+      <c r="W11">
+        <v>12.4069</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -1773,8 +1701,8 @@
       <c r="V16">
         <v>0.0682143534556259</v>
       </c>
-      <c r="W16" t="s">
-        <v>46</v>
+      <c r="W16">
+        <v>411.1219</v>
       </c>
     </row>
     <row r="17" spans="1:25">
@@ -1844,8 +1772,8 @@
       <c r="V17">
         <v>0.113314344354501</v>
       </c>
-      <c r="W17" t="s">
-        <v>47</v>
+      <c r="W17">
+        <v>18.1851</v>
       </c>
     </row>
     <row r="18" spans="1:25">
@@ -2223,8 +2151,8 @@
       <c r="V22">
         <v>0.0382983446945548</v>
       </c>
-      <c r="W22" t="s">
-        <v>48</v>
+      <c r="W22">
+        <v>1439.7406</v>
       </c>
     </row>
     <row r="23" spans="1:25">
@@ -2294,8 +2222,8 @@
       <c r="V23">
         <v>0.07727435862776599</v>
       </c>
-      <c r="W23" t="s">
-        <v>49</v>
+      <c r="W23">
+        <v>33.7482</v>
       </c>
     </row>
     <row r="24" spans="1:25">
@@ -2673,8 +2601,8 @@
       <c r="V28">
         <v>0.0861901419148729</v>
       </c>
-      <c r="W28" t="s">
-        <v>50</v>
+      <c r="W28">
+        <v>997.8453</v>
       </c>
     </row>
     <row r="29" spans="1:25">
@@ -2744,8 +2672,8 @@
       <c r="V29">
         <v>0.1263467683197098</v>
       </c>
-      <c r="W29" t="s">
-        <v>51</v>
+      <c r="W29">
+        <v>27.9478</v>
       </c>
     </row>
     <row r="30" spans="1:25">
@@ -3123,8 +3051,8 @@
       <c r="V34">
         <v>0.5346020107687763</v>
       </c>
-      <c r="W34" t="s">
-        <v>52</v>
+      <c r="W34">
+        <v>69.3459</v>
       </c>
     </row>
     <row r="35" spans="1:25">
@@ -3194,8 +3122,8 @@
       <c r="V35">
         <v>0.555077327499603</v>
       </c>
-      <c r="W35" t="s">
-        <v>53</v>
+      <c r="W35">
+        <v>3.4404</v>
       </c>
     </row>
     <row r="36" spans="1:25">
@@ -3573,8 +3501,8 @@
       <c r="V40">
         <v>0.4689150364546233</v>
       </c>
-      <c r="W40" t="s">
-        <v>54</v>
+      <c r="W40">
+        <v>100.5543</v>
       </c>
     </row>
     <row r="41" spans="1:25">
@@ -3644,8 +3572,8 @@
       <c r="V41">
         <v>0.5209789951845107</v>
       </c>
-      <c r="W41" t="s">
-        <v>55</v>
+      <c r="W41">
+        <v>4.3565</v>
       </c>
     </row>
     <row r="42" spans="1:25">
@@ -4023,8 +3951,8 @@
       <c r="V46">
         <v>0.6374529640958072</v>
       </c>
-      <c r="W46" t="s">
-        <v>56</v>
+      <c r="W46">
+        <v>40.166</v>
       </c>
     </row>
     <row r="47" spans="1:25">
@@ -4094,8 +4022,8 @@
       <c r="V47">
         <v>0.6548904595720243</v>
       </c>
-      <c r="W47" t="s">
-        <v>57</v>
+      <c r="W47">
+        <v>2.481</v>
       </c>
     </row>
     <row r="48" spans="1:25">
@@ -4473,8 +4401,8 @@
       <c r="V52">
         <v>0.531720433279101</v>
       </c>
-      <c r="W52" t="s">
-        <v>58</v>
+      <c r="W52">
+        <v>52.8296</v>
       </c>
     </row>
     <row r="53" spans="1:25">
@@ -4544,8 +4472,8 @@
       <c r="V53">
         <v>0.556397594705997</v>
       </c>
-      <c r="W53" t="s">
-        <v>59</v>
+      <c r="W53">
+        <v>3.4475</v>
       </c>
     </row>
     <row r="54" spans="1:25">
@@ -4923,8 +4851,8 @@
       <c r="V58">
         <v>0.4765033251463078</v>
       </c>
-      <c r="W58" t="s">
-        <v>60</v>
+      <c r="W58">
+        <v>43.1859</v>
       </c>
     </row>
     <row r="59" spans="1:25">
@@ -4994,8 +4922,8 @@
       <c r="V59">
         <v>0.5178639058370467</v>
       </c>
-      <c r="W59" t="s">
-        <v>61</v>
+      <c r="W59">
+        <v>2.1179</v>
       </c>
     </row>
     <row r="60" spans="1:25">
@@ -5373,8 +5301,8 @@
       <c r="V64">
         <v>0.2023499263117841</v>
       </c>
-      <c r="W64" t="s">
-        <v>62</v>
+      <c r="W64">
+        <v>345.8308</v>
       </c>
     </row>
     <row r="65" spans="1:25">
@@ -5444,8 +5372,8 @@
       <c r="V65">
         <v>0.709298940987285</v>
       </c>
-      <c r="W65" t="s">
-        <v>63</v>
+      <c r="W65">
+        <v>5.1412</v>
       </c>
     </row>
     <row r="66" spans="1:25">
@@ -5823,8 +5751,8 @@
       <c r="V70">
         <v>0.0592108657355863</v>
       </c>
-      <c r="W70" t="s">
-        <v>64</v>
+      <c r="W70">
+        <v>386.5587</v>
       </c>
     </row>
     <row r="71" spans="1:25">
@@ -5894,8 +5822,8 @@
       <c r="V71">
         <v>0.1789466618054607</v>
       </c>
-      <c r="W71" t="s">
-        <v>65</v>
+      <c r="W71">
+        <v>4.7858</v>
       </c>
     </row>
     <row r="72" spans="1:25">

</xml_diff>